<commit_message>
implemented number of strike logic
</commit_message>
<xml_diff>
--- a/option_chain_bkp.xlsx
+++ b/option_chain_bkp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb4cecaa05735e09/Desktop/bipinmsit/tradetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC1048C589D870065ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903FC1EA-03A0-4CA8-8CA4-12EE5E29102A}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_F25DC773A252ABDACC1048C589D870065ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60C3CDA1-F0DB-4F2B-AFF3-8C258C3F3671}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,8 @@
   <dimension ref="A1:S106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>